<commit_message>
Adds harmon ranking to team tab and formatting
</commit_message>
<xml_diff>
--- a/data/Reception_Perception_Dynasty.xlsx
+++ b/data/Reception_Perception_Dynasty.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/28a1ee50a88aa706/python_work/Dynasty_tools/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="8_{389A4676-7C93-4697-AA30-3844E99EB7A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B8052AAA-AD6C-4056-B55E-CF23DF8789BC}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="8_{389A4676-7C93-4697-AA30-3844E99EB7A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{61E64332-BF40-4A8A-8A7B-6E13ACCA717F}"/>
   <bookViews>
-    <workbookView xWindow="-310" yWindow="21990" windowWidth="21860" windowHeight="15760" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2660" yWindow="2660" windowWidth="28800" windowHeight="15460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,12 +22,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="257">
   <si>
-    <t>Rank</t>
-  </si>
-  <si>
-    <t>Player</t>
-  </si>
-  <si>
     <t>Draft Year</t>
   </si>
   <si>
@@ -763,9 +757,6 @@
     <t>Not sure what his best position is but has some skills to hang around</t>
   </si>
   <si>
-    <t>Tier</t>
-  </si>
-  <si>
     <t>Prized Dynasty Asset</t>
   </si>
   <si>
@@ -791,6 +782,15 @@
   </si>
   <si>
     <t>Waiver Wire Option</t>
+  </si>
+  <si>
+    <t>Tier_Harmon</t>
+  </si>
+  <si>
+    <t>Player_Harmon</t>
+  </si>
+  <si>
+    <t>Rank_Harmon</t>
   </si>
 </sst>
 </file>
@@ -1177,12 +1177,12 @@
   <dimension ref="A1:F119"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6" customWidth="1"/>
+    <col min="1" max="1" width="11.08984375" customWidth="1"/>
     <col min="2" max="2" width="32.36328125" customWidth="1"/>
     <col min="3" max="3" width="13.453125" customWidth="1"/>
     <col min="4" max="4" width="41.1796875" customWidth="1"/>
@@ -1192,22 +1192,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -1215,19 +1215,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C2" s="2">
         <v>2021</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E2" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="F2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -1235,19 +1235,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C3" s="2">
         <v>2020</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="F3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
@@ -1255,19 +1255,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C4" s="2">
         <v>2020</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="F4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
@@ -1275,19 +1275,19 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C5" s="2">
         <v>2021</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E5" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="F5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -1295,19 +1295,19 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C6" s="2">
         <v>2023</v>
       </c>
       <c r="D6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E6" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="F6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
@@ -1315,19 +1315,19 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C7" s="2">
         <v>2024</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E7" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="F7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
@@ -1335,19 +1335,19 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C8" s="2">
         <v>2021</v>
       </c>
       <c r="D8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E8" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="F8" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
@@ -1355,19 +1355,19 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C9" s="2">
         <v>2022</v>
       </c>
       <c r="D9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E9" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="F9" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
@@ -1375,19 +1375,19 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C10" s="2">
         <v>2024</v>
       </c>
       <c r="D10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E10" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="F10" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
@@ -1395,19 +1395,19 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C11" s="2">
         <v>2022</v>
       </c>
       <c r="D11" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E11" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="F11" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -1415,19 +1415,19 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C12" s="2">
         <v>2019</v>
       </c>
       <c r="D12" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E12" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="F12" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
@@ -1435,19 +1435,19 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C13" s="2">
         <v>2023</v>
       </c>
       <c r="D13" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E13" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="F13" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
@@ -1455,19 +1455,19 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C14" s="2">
         <v>2024</v>
       </c>
       <c r="D14" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E14" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="F14" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
@@ -1475,19 +1475,19 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C15" s="2">
         <v>2024</v>
       </c>
       <c r="D15" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E15" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="F15" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
@@ -1495,19 +1495,19 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C16" s="2">
         <v>2024</v>
       </c>
       <c r="D16" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E16" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="F16" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
@@ -1515,19 +1515,19 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C17" s="2">
         <v>2020</v>
       </c>
       <c r="D17" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E17" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="F17" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
@@ -1535,19 +1535,19 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C18" s="2">
         <v>2020</v>
       </c>
       <c r="D18" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E18" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="F18" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
@@ -1555,19 +1555,19 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C19" s="2">
         <v>2022</v>
       </c>
       <c r="D19" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E19" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="F19" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
@@ -1575,19 +1575,19 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C20" s="2">
         <v>2023</v>
       </c>
       <c r="D20" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E20" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="F20" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
@@ -1595,19 +1595,19 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C21" s="2">
         <v>2023</v>
       </c>
       <c r="D21" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E21" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="F21" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
@@ -1615,19 +1615,19 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C22" s="2">
         <v>2023</v>
       </c>
       <c r="D22" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E22" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="F22" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
@@ -1635,19 +1635,19 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C23" s="2">
         <v>2023</v>
       </c>
       <c r="D23" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E23" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="F23" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
@@ -1655,19 +1655,19 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C24" s="2">
         <v>2019</v>
       </c>
       <c r="D24" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E24" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="F24" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
@@ -1675,19 +1675,19 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C25" s="2">
         <v>2018</v>
       </c>
       <c r="D25" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E25" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="F25" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
@@ -1695,19 +1695,19 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C26" s="2">
         <v>2021</v>
       </c>
       <c r="D26" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E26" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="F26" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
@@ -1715,19 +1715,19 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C27" s="2">
         <v>2021</v>
       </c>
       <c r="D27" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E27" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="F27" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
@@ -1735,19 +1735,19 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C28" s="2">
         <v>2022</v>
       </c>
       <c r="D28" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E28" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="F28" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
@@ -1755,19 +1755,19 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C29" s="2">
         <v>2017</v>
       </c>
       <c r="D29" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E29" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="F29" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
@@ -1775,19 +1775,19 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C30" s="2">
         <v>2023</v>
       </c>
       <c r="D30" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E30" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="F30" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
@@ -1795,19 +1795,19 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C31" s="2">
         <v>2022</v>
       </c>
       <c r="D31" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E31" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="F31" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.35">
@@ -1815,19 +1815,19 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C32" s="2">
         <v>2019</v>
       </c>
       <c r="D32" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E32" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="F32" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
@@ -1835,19 +1835,19 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C33" s="2">
         <v>2020</v>
       </c>
       <c r="D33" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E33" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="F33" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.35">
@@ -1855,19 +1855,19 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C34" s="2">
         <v>2017</v>
       </c>
       <c r="D34" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E34" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="F34" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.35">
@@ -1875,19 +1875,19 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C35" s="2">
         <v>2024</v>
       </c>
       <c r="D35" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E35" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="F35" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
@@ -1895,19 +1895,19 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C36" s="2">
         <v>2014</v>
       </c>
       <c r="D36" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E36" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="F36" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.35">
@@ -1915,19 +1915,19 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C37" s="2">
         <v>2014</v>
       </c>
       <c r="D37" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E37" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="F37" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.35">
@@ -1935,19 +1935,19 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C38" s="2">
         <v>2022</v>
       </c>
       <c r="D38" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E38" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="F38" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.35">
@@ -1955,19 +1955,19 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C39" s="2">
         <v>2018</v>
       </c>
       <c r="D39" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E39" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="F39" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.35">
@@ -1975,19 +1975,19 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C40" s="2">
         <v>2024</v>
       </c>
       <c r="D40" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E40" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="F40" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.35">
@@ -1995,19 +1995,19 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C41" s="2">
         <v>2020</v>
       </c>
       <c r="D41" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E41" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="F41" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.35">
@@ -2015,19 +2015,19 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C42" s="2">
         <v>2015</v>
       </c>
       <c r="D42" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E42" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="F42" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.35">
@@ -2035,19 +2035,19 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C43" s="2">
         <v>2023</v>
       </c>
       <c r="D43" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E43" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="F43" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.35">
@@ -2055,19 +2055,19 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C44" s="2">
         <v>2022</v>
       </c>
       <c r="D44" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E44" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="F44" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.35">
@@ -2075,19 +2075,19 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C45" s="2">
         <v>2019</v>
       </c>
       <c r="D45" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E45" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="F45" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.35">
@@ -2095,19 +2095,19 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C46" s="2">
         <v>2021</v>
       </c>
       <c r="D46" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E46" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="F46" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.35">
@@ -2115,19 +2115,19 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C47" s="2">
         <v>2020</v>
       </c>
       <c r="D47" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E47" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="F47" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.35">
@@ -2135,19 +2135,19 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C48" s="2">
         <v>2017</v>
       </c>
       <c r="D48" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E48" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="F48" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.35">
@@ -2155,19 +2155,19 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C49" s="2">
         <v>2023</v>
       </c>
       <c r="D49" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E49" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="F49" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.35">
@@ -2175,19 +2175,19 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C50" s="2">
         <v>2024</v>
       </c>
       <c r="D50" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E50" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="F50" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.35">
@@ -2195,19 +2195,19 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C51" s="2">
         <v>2024</v>
       </c>
       <c r="D51" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E51" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="F51" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.35">
@@ -2215,19 +2215,19 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C52" s="2">
         <v>2024</v>
       </c>
       <c r="D52" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E52" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="F52" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.35">
@@ -2235,19 +2235,19 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C53" s="2">
         <v>2018</v>
       </c>
       <c r="D53" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E53" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="F53" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.35">
@@ -2255,19 +2255,19 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C54" s="2">
         <v>2019</v>
       </c>
       <c r="D54" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E54" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="F54" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.35">
@@ -2275,19 +2275,19 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C55" s="2">
         <v>2019</v>
       </c>
       <c r="D55" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E55" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="F55" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.35">
@@ -2295,19 +2295,19 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C56" s="2">
         <v>2020</v>
       </c>
       <c r="D56" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E56" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="F56" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.35">
@@ -2315,19 +2315,19 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C57" s="2">
         <v>2022</v>
       </c>
       <c r="D57" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E57" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="F57" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.35">
@@ -2335,19 +2335,19 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C58" s="2">
         <v>2024</v>
       </c>
       <c r="D58" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E58" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="F58" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.35">
@@ -2355,19 +2355,19 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C59" s="2">
         <v>2024</v>
       </c>
       <c r="D59" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E59" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="F59" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.35">
@@ -2375,19 +2375,19 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C60" s="2">
         <v>2015</v>
       </c>
       <c r="D60" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E60" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="F60" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.35">
@@ -2395,19 +2395,19 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C61" s="2">
         <v>2023</v>
       </c>
       <c r="D61" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E61" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="F61" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.35">
@@ -2415,19 +2415,19 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C62" s="2">
         <v>2019</v>
       </c>
       <c r="D62" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E62" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="F62" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.35">
@@ -2435,19 +2435,19 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C63" s="2">
         <v>2018</v>
       </c>
       <c r="D63" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E63" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="F63" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.35">
@@ -2455,19 +2455,19 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C64" s="2">
         <v>2023</v>
       </c>
       <c r="D64" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E64" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="F64" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.35">
@@ -2475,19 +2475,19 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C65" s="2">
         <v>2021</v>
       </c>
       <c r="D65" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E65" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="F65" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.35">
@@ -2495,19 +2495,19 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C66" s="2">
         <v>2023</v>
       </c>
       <c r="D66" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E66" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="F66" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.35">
@@ -2515,19 +2515,19 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C67" s="2">
         <v>2013</v>
       </c>
       <c r="D67" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E67" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="F67" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.35">
@@ -2535,19 +2535,19 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C68" s="2">
         <v>2022</v>
       </c>
       <c r="D68" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E68" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="F68" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.35">
@@ -2555,19 +2555,19 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C69" s="2">
         <v>2024</v>
       </c>
       <c r="D69" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E69" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="F69" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.35">
@@ -2575,19 +2575,19 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C70" s="2">
         <v>2023</v>
       </c>
       <c r="D70" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E70" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="F70" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.35">
@@ -2595,19 +2595,19 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C71" s="2">
         <v>2022</v>
       </c>
       <c r="D71" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E71" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="F71" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.35">
@@ -2615,19 +2615,19 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C72" s="2">
         <v>2022</v>
       </c>
       <c r="D72" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E72" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="F72" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.35">
@@ -2635,19 +2635,19 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C73" s="2">
         <v>2023</v>
       </c>
       <c r="D73" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E73" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="F73" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.35">
@@ -2655,19 +2655,19 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C74" s="2">
         <v>2023</v>
       </c>
       <c r="D74" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E74" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="F74" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.35">
@@ -2675,19 +2675,19 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C75" s="2">
         <v>2024</v>
       </c>
       <c r="D75" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E75" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="F75" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.35">
@@ -2695,19 +2695,19 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C76" s="2">
         <v>2024</v>
       </c>
       <c r="D76" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E76" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="F76" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.35">
@@ -2715,19 +2715,19 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C77" s="2">
         <v>2022</v>
       </c>
       <c r="D77" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E77" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="F77" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.35">
@@ -2735,19 +2735,19 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C78" s="2">
         <v>2023</v>
       </c>
       <c r="D78" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E78" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="F78" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.35">
@@ -2755,19 +2755,19 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C79" s="2">
         <v>2013</v>
       </c>
       <c r="D79" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E79" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="F79" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.35">
@@ -2775,19 +2775,19 @@
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C80" s="2">
         <v>2017</v>
       </c>
       <c r="D80" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E80" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="F80" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.35">
@@ -2795,19 +2795,19 @@
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C81" s="2">
         <v>2024</v>
       </c>
       <c r="D81" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E81" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="F81" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.35">
@@ -2815,19 +2815,19 @@
         <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C82" s="2">
         <v>2013</v>
       </c>
       <c r="D82" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E82" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="F82" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.35">
@@ -2835,19 +2835,19 @@
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C83" s="2">
         <v>2024</v>
       </c>
       <c r="D83" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E83" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="F83" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.35">
@@ -2855,19 +2855,19 @@
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C84" s="2">
         <v>2021</v>
       </c>
       <c r="D84" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E84" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="F84" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.35">
@@ -2875,19 +2875,19 @@
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C85" s="2">
         <v>2024</v>
       </c>
       <c r="D85" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E85" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="F85" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.35">
@@ -2895,19 +2895,19 @@
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C86" s="2">
         <v>2024</v>
       </c>
       <c r="D86" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E86" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="F86" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.35">
@@ -2915,19 +2915,19 @@
         <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C87" s="2">
         <v>2021</v>
       </c>
       <c r="D87" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E87" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="F87" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.35">
@@ -2935,19 +2935,19 @@
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C88" s="2">
         <v>2020</v>
       </c>
       <c r="D88" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E88" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="F88" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.35">
@@ -2955,19 +2955,19 @@
         <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C89" s="2">
         <v>2022</v>
       </c>
       <c r="D89" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E89" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="F89" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.35">
@@ -2975,19 +2975,19 @@
         <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C90" s="2">
         <v>2024</v>
       </c>
       <c r="D90" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E90" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="F90" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.35">
@@ -2995,19 +2995,19 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C91" s="2">
         <v>2015</v>
       </c>
       <c r="D91" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E91" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="F91" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.35">
@@ -3015,19 +3015,19 @@
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C92" s="2">
         <v>2022</v>
       </c>
       <c r="D92" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E92" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="F92" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.35">
@@ -3035,19 +3035,19 @@
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C93" s="2">
         <v>2014</v>
       </c>
       <c r="D93" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E93" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="F93" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.35">
@@ -3055,19 +3055,19 @@
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C94" s="2">
         <v>2023</v>
       </c>
       <c r="D94" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E94" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="F94" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.35">
@@ -3075,19 +3075,19 @@
         <v>94</v>
       </c>
       <c r="B95" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C95" s="2">
         <v>2024</v>
       </c>
       <c r="D95" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E95" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="F95" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.35">
@@ -3095,19 +3095,19 @@
         <v>95</v>
       </c>
       <c r="B96" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C96" s="2">
         <v>2019</v>
       </c>
       <c r="D96" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E96" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="F96" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.35">
@@ -3115,19 +3115,19 @@
         <v>96</v>
       </c>
       <c r="B97" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C97" s="2">
         <v>2019</v>
       </c>
       <c r="D97" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E97" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="F97" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.35">
@@ -3135,19 +3135,19 @@
         <v>97</v>
       </c>
       <c r="B98" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C98" s="2">
         <v>2017</v>
       </c>
       <c r="D98" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E98" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="F98" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.35">
@@ -3155,19 +3155,19 @@
         <v>98</v>
       </c>
       <c r="B99" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C99" s="2">
         <v>2024</v>
       </c>
       <c r="D99" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E99" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="F99" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.35">
@@ -3175,19 +3175,19 @@
         <v>99</v>
       </c>
       <c r="B100" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C100" s="2">
         <v>2024</v>
       </c>
       <c r="D100" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E100" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="F100" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.35">
@@ -3195,19 +3195,19 @@
         <v>100</v>
       </c>
       <c r="B101" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C101" s="2">
         <v>2022</v>
       </c>
       <c r="D101" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E101" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="F101" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.35">
@@ -3215,19 +3215,19 @@
         <v>101</v>
       </c>
       <c r="B102" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C102" s="2">
         <v>2022</v>
       </c>
       <c r="D102" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E102" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="F102" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.35">
@@ -3235,19 +3235,19 @@
         <v>102</v>
       </c>
       <c r="B103" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C103" s="2">
         <v>2022</v>
       </c>
       <c r="D103" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E103" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="F103" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.35">
@@ -3255,19 +3255,19 @@
         <v>103</v>
       </c>
       <c r="B104" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C104" s="2">
         <v>2018</v>
       </c>
       <c r="D104" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="E104" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="F104" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.35">
@@ -3275,19 +3275,19 @@
         <v>104</v>
       </c>
       <c r="B105" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C105" s="2">
         <v>2024</v>
       </c>
       <c r="D105" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E105" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="F105" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.35">
@@ -3295,19 +3295,19 @@
         <v>105</v>
       </c>
       <c r="B106" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C106" s="2">
         <v>2018</v>
       </c>
       <c r="D106" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E106" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="F106" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.35">
@@ -3315,19 +3315,19 @@
         <v>106</v>
       </c>
       <c r="B107" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C107" s="2">
         <v>2020</v>
       </c>
       <c r="D107" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E107" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="F107" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.35">
@@ -3335,19 +3335,19 @@
         <v>107</v>
       </c>
       <c r="B108" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C108" s="2">
         <v>2017</v>
       </c>
       <c r="D108" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="E108" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="F108" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.35">
@@ -3355,19 +3355,19 @@
         <v>108</v>
       </c>
       <c r="B109" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C109" s="2">
         <v>2024</v>
       </c>
       <c r="D109" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E109" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="F109" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.35">
@@ -3375,19 +3375,19 @@
         <v>109</v>
       </c>
       <c r="B110" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C110" s="2">
         <v>2023</v>
       </c>
       <c r="D110" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="E110" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="F110" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.35">
@@ -3395,19 +3395,19 @@
         <v>110</v>
       </c>
       <c r="B111" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C111" s="2">
         <v>2024</v>
       </c>
       <c r="D111" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="E111" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="F111" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.35">
@@ -3415,19 +3415,19 @@
         <v>111</v>
       </c>
       <c r="B112" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C112" s="2">
         <v>2023</v>
       </c>
       <c r="D112" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E112" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="F112" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.35">
@@ -3435,19 +3435,19 @@
         <v>112</v>
       </c>
       <c r="B113" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C113" s="2">
         <v>2016</v>
       </c>
       <c r="D113" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="E113" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="F113" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.35">
@@ -3455,19 +3455,19 @@
         <v>113</v>
       </c>
       <c r="B114" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C114" s="2">
         <v>2017</v>
       </c>
       <c r="D114" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E114" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="F114" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.35">
@@ -3475,19 +3475,19 @@
         <v>114</v>
       </c>
       <c r="B115" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C115" s="2">
         <v>2021</v>
       </c>
       <c r="D115" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="E115" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="F115" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.35">
@@ -3495,19 +3495,19 @@
         <v>115</v>
       </c>
       <c r="B116" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C116" s="2">
         <v>2024</v>
       </c>
       <c r="D116" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E116" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="F116" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.35">
@@ -3515,19 +3515,19 @@
         <v>116</v>
       </c>
       <c r="B117" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C117" s="2">
         <v>2023</v>
       </c>
       <c r="D117" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="E117" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="F117" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.35">
@@ -3535,19 +3535,19 @@
         <v>117</v>
       </c>
       <c r="B118" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C118" s="2">
         <v>2021</v>
       </c>
       <c r="D118" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="E118" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="F118" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.35">
@@ -3555,19 +3555,19 @@
         <v>118</v>
       </c>
       <c r="B119" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C119" s="2">
         <v>2023</v>
       </c>
       <c r="D119" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="E119" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="F119" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>